<commit_message>
Committing as of 13/02/20 10:00 AM
</commit_message>
<xml_diff>
--- a/Urbest/resources/testdata.xlsx
+++ b/Urbest/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t xml:space="preserve">Test Case Name</t>
   </si>
@@ -58,7 +58,19 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Membername</t>
+    <t xml:space="preserve">Member name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
     <t xml:space="preserve">To_verify_if_client_is_able_to_login_to_the_application</t>
@@ -294,10 +306,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,7 +321,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,82 +366,94 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>